<commit_message>
2.3.6: defineAnnotation flag is added to cgInterface for defining original annotation in Java.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCgInterfaceValueObject.xlsx
+++ b/meta/program/BlancoCgInterfaceValueObject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCg/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78909E60-FED0-BD44-8C77-4CC3C44789C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A5C7CB-A7FD-F143-A6A0-2F88F86B7815}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -333,12 +333,36 @@
       <t xml:space="preserve">キジュツ </t>
     </rPh>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>defineAnnotation</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>java.lang.Boolean</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>独自アノテーションを定義するためのインタフェースの場合はtrueを設定してください。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ドクジアノテーショｎ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">テイギスル </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t xml:space="preserve">セッテイシテクダサイ。 </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -897,40 +921,40 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1246,14 +1270,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1320,12 +1344,12 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="62"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
@@ -1426,23 +1450,23 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="58"/>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="54"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="63"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="58"/>
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6">
@@ -1479,29 +1503,29 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="59" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6">
@@ -1539,7 +1563,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="44">
-        <f t="shared" ref="A29:A37" si="0">A28+1</f>
+        <f t="shared" ref="A29:A38" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="45" t="s">
@@ -1568,7 +1592,7 @@
       <c r="D30" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="52" t="s">
         <v>48</v>
       </c>
       <c r="F30" s="53"/>
@@ -1587,7 +1611,7 @@
       <c r="D31" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="58" t="s">
+      <c r="E31" s="52" t="s">
         <v>49</v>
       </c>
       <c r="F31" s="53"/>
@@ -1606,7 +1630,7 @@
       <c r="D32" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="52" t="s">
         <v>50</v>
       </c>
       <c r="F32" s="53"/>
@@ -1625,7 +1649,7 @@
       <c r="D33" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="52" t="s">
         <v>51</v>
       </c>
       <c r="F33" s="53"/>
@@ -1644,7 +1668,7 @@
       <c r="D34" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="58" t="s">
+      <c r="E34" s="52" t="s">
         <v>52</v>
       </c>
       <c r="F34" s="53"/>
@@ -1672,7 +1696,7 @@
         <v>44</v>
       </c>
       <c r="D36" s="24"/>
-      <c r="E36" s="59" t="s">
+      <c r="E36" s="54" t="s">
         <v>53</v>
       </c>
       <c r="F36" s="53"/>
@@ -1691,29 +1715,59 @@
       <c r="D37" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="52" t="s">
+      <c r="E37" s="60" t="s">
         <v>66</v>
       </c>
       <c r="F37" s="53"/>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="25"/>
+    <row r="38" spans="1:6" s="51" customFormat="1" ht="35" customHeight="1">
+      <c r="A38" s="48">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="53"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="26"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="29"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="C8:F8"/>
@@ -1722,36 +1776,26 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D55">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D56" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1764,7 +1808,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>